<commit_message>
Write the number of lettre in the _freq text
</commit_message>
<xml_diff>
--- a/Avancement.xlsx
+++ b/Avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\eclipse-workspace\Code de Huffman\src\codageHuffman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C665679-BADF-43D4-B044-027878E63DAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8341486E-2AAD-4DDE-BD23-907C3BF01DAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="24120" windowHeight="15435" xr2:uid="{0E1C7E2E-5928-4CBE-9D68-D5FA26EC4BA6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Tache</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Déterminer et afficher le nombre moyen de bits de stockage d’un caractère dans le texte codé</t>
+  </si>
+  <si>
+    <t>Branch</t>
   </si>
 </sst>
 </file>
@@ -114,11 +117,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,11 +135,11 @@
   <dxfs count="6">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -146,21 +155,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -178,6 +177,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -491,97 +500,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490ADD04-9DCC-48DD-A6E3-9902E9ABDCA9}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.7109375" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="11.42578125" style="5"/>
+    <col min="2" max="2" width="84.7109375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"En cours"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Fait"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"En cours"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
+  <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"En cours"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"En cours"</formula>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Non fait"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Fait"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Non fait"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"En cours"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>